<commit_message>
Working passing user as arg
</commit_message>
<xml_diff>
--- a/python/exel/goscie.xlsx
+++ b/python/exel/goscie.xlsx
@@ -397,17 +397,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Tomek</v>
+        <v>Nick</v>
       </c>
       <c r="B1" t="str">
-        <v>123</v>
+        <v>Password</v>
       </c>
     </row>
     <row r="2">
@@ -426,9 +426,17 @@
         <v>789</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Tomek</v>
+      </c>
+      <c r="B4" t="str">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Problem in changing value of sending link in goscie.xlsx
</commit_message>
<xml_diff>
--- a/python/exel/goscie.xlsx
+++ b/python/exel/goscie.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -409,6 +409,9 @@
       <c r="B1" t="str">
         <v>Password</v>
       </c>
+      <c r="C1" t="str">
+        <v>Send</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -417,6 +420,12 @@
       <c r="B2" t="str">
         <v>456</v>
       </c>
+      <c r="C2" t="str">
+        <v>No</v>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -425,6 +434,9 @@
       <c r="B3" t="str">
         <v>789</v>
       </c>
+      <c r="C3" t="str">
+        <v>No</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -433,10 +445,13 @@
       <c r="B4" t="str">
         <v>123</v>
       </c>
+      <c r="C4" t="str">
+        <v>No</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>